<commit_message>
resolving issues with excel master file
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,28 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexandra.veizu\Documents\Reframework_update_UiPath_Services\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\Projects\Client Projects\eShopWorld\Processes\ESWNikeDailyRefunds\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE7DFF5-5AFC-4110-8461-609B0BDD5551}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2D8DE8-C588-4DD2-9E98-99E4B7D67787}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-45" yWindow="-18120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="64">
   <si>
     <t>Name</t>
   </si>
@@ -85,13 +96,6 @@
   </si>
   <si>
     <t>logF_BusinessProcessName</t>
-  </si>
-  <si>
-    <t>Framework</t>
-  </si>
-  <si>
-    <t>ProcessABCQueue</t>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
@@ -122,13 +126,115 @@
   </si>
   <si>
     <t>OrchestratorAssetFolder</t>
+  </si>
+  <si>
+    <t>OrchestratorFolderPath</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>ESWNikeDailyRefunds</t>
+  </si>
+  <si>
+    <t>C:\ESW\CustomerService2013\VSD\Refunds\Refund Files\Nike\{year}</t>
+  </si>
+  <si>
+    <t>RefundMasterFolderPath</t>
+  </si>
+  <si>
+    <t>RefundMasterFile</t>
+  </si>
+  <si>
+    <t>DailyFraudFile</t>
+  </si>
+  <si>
+    <t>{month} {year} Nike Master Refunds.xlsb</t>
+  </si>
+  <si>
+    <t>eCommerce Refund Report {date}.xlsx</t>
+  </si>
+  <si>
+    <t>CSPRootUrl</t>
+  </si>
+  <si>
+    <t>CSPLoginUrlPath</t>
+  </si>
+  <si>
+    <t>Account/Login</t>
+  </si>
+  <si>
+    <t>CSPSearchFinTransUrlPath</t>
+  </si>
+  <si>
+    <t>Finance/Transaction/FinTranApproval</t>
+  </si>
+  <si>
+    <t>BrowserProcessName</t>
+  </si>
+  <si>
+    <t>chrome.exe</t>
+  </si>
+  <si>
+    <t>This is the process name of the browser to be used for web applications [Chrome -&gt; chrome.exe, MS Edge -&gt; msedge.exe, Firefox -&gt; firefox.exe, IE -&gt; iexplore.exe]</t>
+  </si>
+  <si>
+    <t>CSPCredentialsAsset</t>
+  </si>
+  <si>
+    <t>TransactionType</t>
+  </si>
+  <si>
+    <t>Refund</t>
+  </si>
+  <si>
+    <t>MaxPageSize</t>
+  </si>
+  <si>
+    <t>AuthorisationStatuses</t>
+  </si>
+  <si>
+    <t>2 -&gt; Pending, 4 -&gt; Authorised, 8 -&gt; Rejected. Bitwise operation so can be combined with pipe symbol to form an inclusion of more then one status</t>
+  </si>
+  <si>
+    <t>ApprovalType</t>
+  </si>
+  <si>
+    <t>Authorise</t>
+  </si>
+  <si>
+    <t>SelectAllTransactions</t>
+  </si>
+  <si>
+    <t>FromDate</t>
+  </si>
+  <si>
+    <t>ToDate</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>Brand</t>
+  </si>
+  <si>
+    <t>Nike</t>
+  </si>
+  <si>
+    <t>https://preprod-csp.nike.eshopworld.net/</t>
+  </si>
+  <si>
+    <t>ESWNikeCSPCredentials</t>
+  </si>
+  <si>
+    <t>08/01/2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -152,6 +258,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -170,10 +282,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -183,8 +296,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -499,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -547,55 +664,176 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>22</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+    </row>
     <row r="4" spans="1:26" ht="30">
       <c r="A4" t="s">
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="7"/>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -1563,8 +1801,11 @@
     <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B10" r:id="rId1" xr:uid="{4CD738E5-0B91-4C67-B908-3C918FD0FA7E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1624,7 +1865,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1648,7 +1889,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -1670,7 +1911,7 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -1681,7 +1922,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1692,7 +1933,7 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2682,7 +2923,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
@@ -2702,7 +2943,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Ready for UAT testing
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\Projects\Client Projects\eShopWorld\Processes\ESWNikeDailyRefunds\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2D8DE8-C588-4DD2-9E98-99E4B7D67787}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F347FAD1-F4E8-4374-913A-3246764CECE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-45" yWindow="-18120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="65">
   <si>
     <t>Name</t>
   </si>
@@ -228,6 +228,9 @@
   </si>
   <si>
     <t>08/01/2020</t>
+  </si>
+  <si>
+    <t>MaxPageRuns</t>
   </si>
 </sst>
 </file>
@@ -614,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -785,46 +788,53 @@
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="B18">
-        <v>2</v>
-      </c>
-      <c r="C18" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19" t="s">
-        <v>54</v>
+        <v>51</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>58</v>
+        <v>53</v>
+      </c>
+      <c r="B20" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A23" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="7"/>
+      <c r="B23" s="7"/>
     </row>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
@@ -1799,6 +1809,7 @@
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
+    <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Send Mail activity added to send transaction audit file to distrinution list
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\Projects\Client Projects\eShopWorld\Processes\ESWNikeDailyRefunds\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hpatel\Documents\UiPath\ESWNikeDailyRefunds\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA50A1D-794E-417A-B451-64CD4DEF7192}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2FA070-8667-4C81-B50B-3235AE521A5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -658,7 +658,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -851,7 +851,7 @@
         <v>59</v>
       </c>
       <c r="B20">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
Resolved Fraud Issue and Added re-implemented CSP Library
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hpatel\Documents\UiPath\ESWNikeDailyRefunds\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\Projects\Client Projects\eShopWorld\Processes\ESWNikeDailyRefunds\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2FA070-8667-4C81-B50B-3235AE521A5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D65D35E-AD7D-483C-BFE8-1D9E4E3E76D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="88">
   <si>
     <t>Name</t>
   </si>
@@ -266,6 +266,39 @@
   </si>
   <si>
     <t>GenerateAuditFile</t>
+  </si>
+  <si>
+    <t>ConsoleToDateDelay</t>
+  </si>
+  <si>
+    <t>The amount in milliseconds to delay between opening the browser console and entering the jquery statement to update the to and from dates.</t>
+  </si>
+  <si>
+    <t>The phrase to search in the master file for potential fraud transactions</t>
+  </si>
+  <si>
+    <t>The phrase to search in the master file for potential do not process transactions</t>
+  </si>
+  <si>
+    <t>Location of Nike Daily Refund Master File</t>
+  </si>
+  <si>
+    <t>The format of Nike Refund Master File</t>
+  </si>
+  <si>
+    <t>The location of the UAT Transactions Audit File</t>
+  </si>
+  <si>
+    <t>The location of the Daily Fraud File</t>
+  </si>
+  <si>
+    <t>Root Url to CSP</t>
+  </si>
+  <si>
+    <t>Relative url path to search financial transactions page</t>
+  </si>
+  <si>
+    <t>Relative url path to Login Page</t>
   </si>
 </sst>
 </file>
@@ -658,7 +691,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -739,6 +772,9 @@
       <c r="B6" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="C6" s="3" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="2" t="s">
@@ -747,6 +783,9 @@
       <c r="B7" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="C7" s="3" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="2" t="s">
@@ -755,6 +794,9 @@
       <c r="B8" s="2" t="s">
         <v>62</v>
       </c>
+      <c r="C8" s="3" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="2" t="s">
@@ -762,6 +804,9 @@
       </c>
       <c r="B9" s="2" t="s">
         <v>71</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
@@ -772,6 +817,9 @@
       <c r="B11" s="6" t="s">
         <v>56</v>
       </c>
+      <c r="C11" s="3" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
@@ -780,6 +828,9 @@
       <c r="B12" t="s">
         <v>40</v>
       </c>
+      <c r="C12" s="3" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
@@ -788,6 +839,9 @@
       <c r="B13" t="s">
         <v>42</v>
       </c>
+      <c r="C13" s="3" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="14" spans="1:26" ht="30">
       <c r="A14" t="s">
@@ -895,6 +949,9 @@
       <c r="B24" t="s">
         <v>64</v>
       </c>
+      <c r="C24" s="3" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
@@ -903,6 +960,9 @@
       <c r="B25" t="s">
         <v>66</v>
       </c>
+      <c r="C25" s="3" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
@@ -928,7 +988,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A29" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29">
+        <v>500</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="32" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Removed browser config item and adjust KillProcess
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\Projects\Client Projects\eShopWorld\Processes\ESWNikeDailyRefunds\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D65D35E-AD7D-483C-BFE8-1D9E4E3E76D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0A146C-5B0F-49D9-AA82-B6753F688D6E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="85">
   <si>
     <t>Name</t>
   </si>
@@ -164,15 +164,6 @@
   </si>
   <si>
     <t>Finance/Transaction/FinTranApproval</t>
-  </si>
-  <si>
-    <t>BrowserProcessName</t>
-  </si>
-  <si>
-    <t>chrome.exe</t>
-  </si>
-  <si>
-    <t>This is the process name of the browser to be used for web applications [Chrome -&gt; chrome.exe, MS Edge -&gt; msedge.exe, Firefox -&gt; firefox.exe, IE -&gt; iexplore.exe]</t>
   </si>
   <si>
     <t>CSPCredentialsAsset</t>
@@ -688,7 +679,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
@@ -773,7 +764,7 @@
         <v>33</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -784,18 +775,18 @@
         <v>37</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -803,10 +794,10 @@
         <v>36</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
@@ -815,10 +806,10 @@
         <v>38</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
@@ -829,7 +820,7 @@
         <v>40</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
@@ -840,165 +831,155 @@
         <v>42</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="30">
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
         <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" t="s">
-        <v>48</v>
+      <c r="A16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="14.25" customHeight="1">
+    <row r="17" spans="1:3" ht="30">
       <c r="A17" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>55</v>
+        <v>65</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="30">
-      <c r="A18" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B18" s="2">
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="30">
+      <c r="A19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19">
         <v>1</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19">
-        <v>5</v>
-      </c>
       <c r="C19" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="30">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30">
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21">
-        <v>2</v>
+        <v>49</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="7"/>
+      <c r="C22" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" s="7"/>
+        <v>60</v>
+      </c>
+      <c r="B23" t="s">
+        <v>61</v>
+      </c>
       <c r="C23" s="3" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" t="s">
         <v>63</v>
       </c>
-      <c r="B24" t="s">
-        <v>64</v>
-      </c>
       <c r="C24" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B25" t="s">
-        <v>66</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B26" t="s">
-        <v>74</v>
-      </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
         <v>73</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>75</v>
+      <c r="B27">
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>500</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A29" t="s">
-        <v>77</v>
-      </c>
-      <c r="B29">
-        <v>500</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
@@ -1967,7 +1948,6 @@
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Impleented sending email on exceptions
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\Projects\Client Projects\eShopWorld\Processes\ESWNikeDailyRefunds\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0A146C-5B0F-49D9-AA82-B6753F688D6E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56AB3C53-FC06-4E16-B6BF-165CC52C6542}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4260" yWindow="1125" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="89">
   <si>
     <t>Name</t>
   </si>
@@ -244,12 +244,6 @@
     <t>C:\ESW\CustomerService2013\VSD\Refunds\Refund Files\Nike\Daily Lookup Files\eCommerce Refund Report.xlsx</t>
   </si>
   <si>
-    <t>EmailSubject</t>
-  </si>
-  <si>
-    <t>EmailBody</t>
-  </si>
-  <si>
     <t>Nike daily refunds Transactions Audit</t>
   </si>
   <si>
@@ -290,6 +284,24 @@
   </si>
   <si>
     <t>Relative url path to Login Page</t>
+  </si>
+  <si>
+    <t>ProcessCompletedEmailSubject</t>
+  </si>
+  <si>
+    <t>ProcessComepletedEmailBody</t>
+  </si>
+  <si>
+    <t>BusinessRuleExceptionEmailSubject</t>
+  </si>
+  <si>
+    <t>Nike Daily Refunds: Business Rule Violation Occurred</t>
+  </si>
+  <si>
+    <t>SystemExceptionEmailSubject</t>
+  </si>
+  <si>
+    <t>Nike Daily Refunds: Exception Occurred</t>
   </si>
 </sst>
 </file>
@@ -679,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -764,7 +776,7 @@
         <v>33</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -775,7 +787,7 @@
         <v>37</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -786,7 +798,7 @@
         <v>59</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -797,7 +809,7 @@
         <v>68</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
@@ -809,7 +821,7 @@
         <v>53</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
@@ -820,7 +832,7 @@
         <v>40</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
@@ -831,7 +843,7 @@
         <v>42</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
@@ -930,7 +942,7 @@
         <v>61</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
@@ -941,64 +953,77 @@
         <v>63</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A25" t="s">
-        <v>69</v>
-      </c>
-      <c r="B25" t="s">
+    <row r="26" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A26" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
-        <v>70</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>72</v>
+      <c r="B26">
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27">
+        <v>500</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
     </row>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A28" t="s">
-        <v>74</v>
-      </c>
-      <c r="B28">
-        <v>500</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>75</v>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A29" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" t="s">
+        <v>69</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A32" t="s">
+        <v>85</v>
+      </c>
+      <c r="B32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A33" t="s">
+        <v>87</v>
+      </c>
+      <c r="B33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="35" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="36" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="37" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="38" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="39" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="40" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="42" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="43" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="44" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="45" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="46" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="48" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>
@@ -1947,7 +1972,6 @@
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Added email support on exceptions
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\Projects\Client Projects\eShopWorld\Processes\ESWNikeDailyRefunds\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56AB3C53-FC06-4E16-B6BF-165CC52C6542}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE0DF0A-2B4D-4CAC-9E1A-8CE8889EFDEE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="1125" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="90">
   <si>
     <t>Name</t>
   </si>
@@ -238,9 +238,6 @@
     <t xml:space="preserve">The maximum number of pages to process, if set to 0 all pages will be processed. This is primarily for UAT testing </t>
   </si>
   <si>
-    <t xml:space="preserve">Force the page size irregardless if the returned number of transactions are greater then the pagesize set. This is primarily for UAT testing </t>
-  </si>
-  <si>
     <t>C:\ESW\CustomerService2013\VSD\Refunds\Refund Files\Nike\Daily Lookup Files\eCommerce Refund Report.xlsx</t>
   </si>
   <si>
@@ -302,6 +299,12 @@
   </si>
   <si>
     <t>Nike Daily Refunds: Exception Occurred</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boolean to f orce the page size irregardless if the returned number of transactions are greater then the pagesize set. This is primarily for UAT testing </t>
+  </si>
+  <si>
+    <t>Boolean to specify if the audit file is to be generated</t>
   </si>
 </sst>
 </file>
@@ -360,21 +363,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -694,319 +714,323 @@
   <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="105.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" style="3" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="105.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" style="8" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" style="5" customWidth="1"/>
+    <col min="27" max="16384" width="14.42578125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
     </row>
     <row r="2" spans="1:26" ht="30">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:26">
-      <c r="A3" t="s">
+      <c r="A3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="30">
-      <c r="A4" t="s">
+      <c r="A4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>76</v>
+      <c r="C6" s="8" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>77</v>
+      <c r="C7" s="8" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>78</v>
+      <c r="C8" s="8" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>79</v>
+      <c r="B9" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" t="s">
+      <c r="A11" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>80</v>
+      <c r="C11" s="8" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" t="s">
+      <c r="A12" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>82</v>
+      <c r="C12" s="8" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" t="s">
+      <c r="A13" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>81</v>
+      <c r="C13" s="8" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" t="s">
+      <c r="A14" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" t="s">
+      <c r="A15" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="5" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="6" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="6">
         <v>1</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>67</v>
+      <c r="C17" s="8" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" t="s">
+      <c r="A18" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="5">
         <v>5</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="8" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="30">
-      <c r="A19" t="s">
+      <c r="A19" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="5">
         <v>1</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="8" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="30">
-      <c r="A20" t="s">
+      <c r="A20" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="5">
         <v>2</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="8" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A21" t="s">
+      <c r="A21" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="8" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A22" t="s">
+      <c r="A22" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="3" t="s">
+      <c r="B22" s="11"/>
+      <c r="C22" s="8" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A23" t="s">
+      <c r="A23" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>74</v>
+      <c r="C23" s="8" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A24" t="s">
+      <c r="A24" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>75</v>
+      <c r="C24" s="8" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A26" t="s">
-        <v>71</v>
-      </c>
-      <c r="B26">
+      <c r="A26" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" s="5">
         <v>1</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A27" t="s">
+      <c r="A27" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="5">
+        <v>400</v>
+      </c>
+      <c r="C27" s="8" t="s">
         <v>72</v>
-      </c>
-      <c r="B27">
-        <v>500</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A29" t="s">
-        <v>83</v>
-      </c>
-      <c r="B29" t="s">
-        <v>69</v>
+      <c r="A29" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" t="s">
-        <v>84</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>70</v>
+      <c r="A30" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A32" t="s">
+      <c r="A32" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="B32" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A33" t="s">
+      <c r="A33" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="B33" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1"/>
@@ -2037,7 +2061,7 @@
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Resolved issues found in issues log as of 06/01/2021
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hpatel\Documents\UiPath\ESWNikeDailyRefunds\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\Projects\Client Projects\eShopWorld\Processes\ESWNikeDailyRefunds\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87606A91-A78B-4C1B-BC03-C40441B304FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5773FA27-9EB2-4560-9202-544E8B544A24}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -202,9 +202,6 @@
     <t>ESWNikeCSPCredentials</t>
   </si>
   <si>
-    <t>08/01/2020</t>
-  </si>
-  <si>
     <t>MaxPageRuns</t>
   </si>
   <si>
@@ -220,9 +217,6 @@
     <t>FraudPhrase</t>
   </si>
   <si>
-    <t>Fraud</t>
-  </si>
-  <si>
     <t>BankDetailsChangedPhrase</t>
   </si>
   <si>
@@ -305,6 +299,12 @@
   </si>
   <si>
     <t>Boolean to specify if the audit file is to be generated</t>
+  </si>
+  <si>
+    <t>fraud</t>
+  </si>
+  <si>
+    <t>04/01/2018</t>
   </si>
 </sst>
 </file>
@@ -713,8 +713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -797,7 +797,7 @@
         <v>33</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -808,18 +808,18 @@
         <v>37</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -827,10 +827,10 @@
         <v>36</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
@@ -842,7 +842,7 @@
         <v>53</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
@@ -853,7 +853,7 @@
         <v>40</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
@@ -864,7 +864,7 @@
         <v>42</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
@@ -893,13 +893,13 @@
     </row>
     <row r="17" spans="1:3" ht="30">
       <c r="A17" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B17" s="6">
         <v>1</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -910,18 +910,18 @@
         <v>5</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="30">
       <c r="A19" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B19" s="5">
         <v>1</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="30">
@@ -940,10 +940,10 @@
         <v>49</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>55</v>
+        <v>89</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
@@ -952,85 +952,85 @@
       </c>
       <c r="B22" s="11"/>
       <c r="C22" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B26" s="5">
         <v>1</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B27" s="5">
         <v>1000</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
       <c r="A32" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1">
       <c r="A33" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Resolved Formula Issue, by adding StudioX WriteCell
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\Projects\Client Projects\eShopWorld\Processes\ESWNikeDailyRefunds\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\Projects\Client Projects\eShopWorld\Processes\VB\ESWNikeDailyRefunds\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5773FA27-9EB2-4560-9202-544E8B544A24}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2816CFF-B288-4F9D-996A-3F497D9C165C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -714,7 +714,7 @@
   <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -993,7 +993,7 @@
         <v>69</v>
       </c>
       <c r="B27" s="5">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
Resolved issue with bot not running
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\Projects\Client Projects\eShopWorld\Processes\VB\ESWNikeDailyRefunds\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hpatel\Documents\UiPath\ESWNikeDailyRefunds\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2816CFF-B288-4F9D-996A-3F497D9C165C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF08A0C-9389-4266-869F-E3347D0B3691}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -714,7 +714,7 @@
   <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -993,7 +993,7 @@
         <v>69</v>
       </c>
       <c r="B27" s="5">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
Implemented CR 1. And update audit file to be create monthly
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hpatel\Documents\UiPath\ESWNikeDailyRefunds\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF08A0C-9389-4266-869F-E3347D0B3691}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2A1D61-2B0F-4BBD-BE75-358421721BE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="92">
   <si>
     <t>Name</t>
   </si>
@@ -211,9 +211,6 @@
     <t>Not required in prod but is needed for UAT</t>
   </si>
   <si>
-    <t>C:\ESW\Audit\Audit_NikeDailyRefund_Transactions.xlsx</t>
-  </si>
-  <si>
     <t>FraudPhrase</t>
   </si>
   <si>
@@ -304,7 +301,16 @@
     <t>fraud</t>
   </si>
   <si>
-    <t>04/01/2018</t>
+    <t>NikeCODMasterCredentialsAsset</t>
+  </si>
+  <si>
+    <t>NikeCODMasterPassword</t>
+  </si>
+  <si>
+    <t>C:\ESW\Audit\Nike Daily\{year}\{month} Audit NikeDailyRefund Transactions.xlsx</t>
+  </si>
+  <si>
+    <t>01/01/2020</t>
   </si>
 </sst>
 </file>
@@ -711,10 +717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z996"/>
+  <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -797,7 +803,7 @@
         <v>33</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -808,7 +814,7 @@
         <v>37</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -816,10 +822,10 @@
         <v>56</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>58</v>
+        <v>90</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -827,10 +833,10 @@
         <v>36</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
@@ -842,7 +848,7 @@
         <v>53</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
@@ -853,7 +859,7 @@
         <v>40</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
@@ -864,7 +870,7 @@
         <v>42</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
@@ -877,163 +883,170 @@
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="5" t="s">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>45</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A17" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B17" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30">
-      <c r="A17" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B17" s="6">
+    <row r="18" spans="1:3" ht="30">
+      <c r="A18" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="6">
         <v>1</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>86</v>
+      <c r="C18" s="8" t="s">
+        <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="5" t="s">
+    <row r="19" spans="1:3">
+      <c r="A19" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B19" s="5">
         <v>5</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="30">
-      <c r="A19" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B19" s="5">
-        <v>1</v>
-      </c>
       <c r="C19" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="30">
       <c r="A20" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="5">
+        <v>1</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="30">
+      <c r="A21" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B21" s="5">
         <v>2</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C21" s="8" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A21" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B22" s="11"/>
+        <v>49</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="C22" s="8" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>88</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="B23" s="11"/>
       <c r="C23" s="8" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A25" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A26" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B26" s="5">
-        <v>1</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>87</v>
+      <c r="C25" s="8" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" s="5">
+        <v>1</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A28" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="5">
+        <v>1000</v>
+      </c>
+      <c r="C28" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B27" s="5">
-        <v>1000</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>70</v>
-      </c>
     </row>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A29" s="5" t="s">
+    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A30" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B31" s="8" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A32" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" spans="1:2" ht="14.25" customHeight="1">
       <c r="A33" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A34" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>85</v>
-      </c>
     </row>
-    <row r="34" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="35" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="36" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="37" spans="1:2" ht="14.25" customHeight="1"/>
@@ -1996,6 +2009,7 @@
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
+    <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Added updated CSP Library reference
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\Projects\Client Projects\eShopWorld\Processes\VB\ESWNikeDailyRefunds\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D040AC-AD38-4250-B83B-FFE3065C5F46}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4B1F1C-4470-43B5-AD75-36A0A4AAD0EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-18120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -732,7 +732,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Made changes to config
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\Projects\Client Projects\eShopWorld\Processes\VB\ESWNikeDailyRefunds\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hpatel\Documents\UiPath\ESWNikeDailyRefunds\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4B1F1C-4470-43B5-AD75-36A0A4AAD0EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41AD58F6-C126-4424-BC1E-06B50B6AB2D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -732,7 +732,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>